<commit_message>
I cleaned the source code
I cleaned the source code and renamed different methods
</commit_message>
<xml_diff>
--- a/dataBase/myTest.xlsx
+++ b/dataBase/myTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toshiba\Desktop\Team_Work\dataBase\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -46,12 +46,22 @@
   </si>
   <si>
     <t>gacko</t>
+  </si>
+  <si>
+    <t>bobi</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ivana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,9 +382,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -475,6 +485,76 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>